<commit_message>
ran DRC, fixed errors, generated gerbers, generated BOM
</commit_message>
<xml_diff>
--- a/manufacturing files/bitcrane BOM.xlsx
+++ b/manufacturing files/bitcrane BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skot/Work/Bitcoin/bitcrane/manufacturing files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skot/Work/Bitcoin/bitcrane/PCB/manufacturing files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B41DB6-A3DA-F84E-B6A6-C82598EB544B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E42D2A-EB6A-F54F-8331-994506F7AA55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="23040" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="23840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="126">
   <si>
     <t>Qty</t>
   </si>
@@ -38,16 +38,19 @@
     <t>PARTNO</t>
   </si>
   <si>
+    <t>DNP</t>
+  </si>
+  <si>
     <t>C1, C2</t>
   </si>
   <si>
     <t>27pf</t>
   </si>
   <si>
-    <t>1292-1291-1-ND</t>
-  </si>
-  <si>
-    <t>0402N270J250CT</t>
+    <t>1276-2622-1-ND</t>
+  </si>
+  <si>
+    <t>CL21C270JCANNNC</t>
   </si>
   <si>
     <t>C3</t>
@@ -56,24 +59,18 @@
     <t>0.1uF 100V</t>
   </si>
   <si>
-    <t>490-10458-1-ND</t>
-  </si>
-  <si>
-    <t>GRM155R62A104KE14D</t>
-  </si>
-  <si>
-    <t>C4, C9, C10, C11, C12, C13, C14, C15, C16, C17, C20</t>
+    <t>1276-6840-1-ND</t>
+  </si>
+  <si>
+    <t>CL21B104KCFNNNE</t>
+  </si>
+  <si>
+    <t>C4, C9, C10, C11, C12, C13, C14, C15, C16, C17, C20, C21</t>
   </si>
   <si>
     <t>0.1uF</t>
   </si>
   <si>
-    <t>478-KGM05AR71C104KHCT-ND</t>
-  </si>
-  <si>
-    <t>KGM05AR71C104KH</t>
-  </si>
-  <si>
     <t>C5</t>
   </si>
   <si>
@@ -104,10 +101,10 @@
     <t>1uF</t>
   </si>
   <si>
-    <t>587-5514-1-ND</t>
-  </si>
-  <si>
-    <t>EMK105BJ105MV-F</t>
+    <t>1276-1066-1-ND</t>
+  </si>
+  <si>
+    <t>CL21B105KAFNNNE</t>
   </si>
   <si>
     <t>C18, C19</t>
@@ -161,9 +158,6 @@
     <t>Hashboard0</t>
   </si>
   <si>
-    <t>455-B18B-PHDSS-ND</t>
-  </si>
-  <si>
     <t>X2026WV-2x09D-46SN</t>
   </si>
   <si>
@@ -176,7 +170,7 @@
     <t>WM10869-ND</t>
   </si>
   <si>
-    <t>J4, J5, J9, J10</t>
+    <t>J4, J5, J6, J7</t>
   </si>
   <si>
     <t>61900411021</t>
@@ -185,7 +179,7 @@
     <t>732-2701-ND</t>
   </si>
   <si>
-    <t>J6</t>
+    <t>J8</t>
   </si>
   <si>
     <t>USB_C_Receptacle_USB2.0</t>
@@ -197,7 +191,19 @@
     <t>USB4105-GF-A</t>
   </si>
   <si>
-    <t>J7, J8</t>
+    <t>J9</t>
+  </si>
+  <si>
+    <t>Hashboard1</t>
+  </si>
+  <si>
+    <t>J10</t>
+  </si>
+  <si>
+    <t>Hashboard2</t>
+  </si>
+  <si>
+    <t>J14, J15, J16, J17</t>
   </si>
   <si>
     <t>0353180420</t>
@@ -215,16 +221,16 @@
     <t>DMP3013SFV-7DICT-ND</t>
   </si>
   <si>
-    <t>R1, R2, R3</t>
+    <t>R1, R2, R3, R20, R21, R24, R25, R26, R27, R28, R29, R39, R40, R41, R42, R43, R44, R45, R46</t>
   </si>
   <si>
     <t>4.7K</t>
   </si>
   <si>
-    <t>311-4.7KLRCT-ND</t>
-  </si>
-  <si>
-    <t>RC0402FR-074K7L</t>
+    <t>311-4.70KCRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0805FR-074K7L</t>
   </si>
   <si>
     <t>R4, R5</t>
@@ -233,10 +239,10 @@
     <t>5.1K</t>
   </si>
   <si>
-    <t>RMCF0402JT5K10CT-ND</t>
-  </si>
-  <si>
-    <t>RMCF0402JT5K10</t>
+    <t>311-5.10KCRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0805FR-075K1L</t>
   </si>
   <si>
     <t>R6</t>
@@ -245,10 +251,10 @@
     <t>2.2K</t>
   </si>
   <si>
-    <t>311-2.20KLRCT-ND</t>
-  </si>
-  <si>
-    <t>RC0402FR-072K2L</t>
+    <t>RMCF0805FT2K20CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0805FT2K20</t>
   </si>
   <si>
     <t>R7, R8, R9</t>
@@ -257,10 +263,10 @@
     <t>10K</t>
   </si>
   <si>
-    <t>RMCF0402FT10K0CT-ND</t>
-  </si>
-  <si>
-    <t>RMCF0402FT10K0</t>
+    <t>RMCF0805FT10K0CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0805FT10K0</t>
   </si>
   <si>
     <t>R10, R12</t>
@@ -269,7 +275,10 @@
     <t>12K</t>
   </si>
   <si>
-    <t>RC0402FR-1312KL</t>
+    <t>RMCF0805FT12K0CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0805FT12K0</t>
   </si>
   <si>
     <t>R11</t>
@@ -278,10 +287,10 @@
     <t>1K</t>
   </si>
   <si>
-    <t>311-1.00KLRCT-ND</t>
-  </si>
-  <si>
-    <t>RC0402FR-071KL</t>
+    <t>RMCF0805FT1K00CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0805FT1K00</t>
   </si>
   <si>
     <t>R13, R14, R15, R16</t>
@@ -290,21 +299,57 @@
     <t>36K</t>
   </si>
   <si>
-    <t>CR0402-FX-3602GLFCT-ND</t>
-  </si>
-  <si>
-    <t>CR0402-FX-3602GLF</t>
+    <t>311-36.0KCRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0805FR-0736KL</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>33k</t>
+  </si>
+  <si>
+    <t>311-33.0KCRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0805FR-0733KL</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>22k</t>
+  </si>
+  <si>
+    <t>RMCF0805FT22K0CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0805FT22K0</t>
+  </si>
+  <si>
+    <t>R19</t>
+  </si>
+  <si>
+    <t>4.7k</t>
+  </si>
+  <si>
+    <t>R30, R31, R32, R33, R34, R35, R36, R37, R38</t>
   </si>
   <si>
     <t>U1</t>
   </si>
   <si>
+    <t>FT4232HQ</t>
+  </si>
+  <si>
+    <t>768-1027-1-ND</t>
+  </si>
+  <si>
     <t>FT4232HQ-REEL</t>
   </si>
   <si>
-    <t>768-1027-1-ND</t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
@@ -326,10 +371,22 @@
     <t>U4</t>
   </si>
   <si>
+    <t>EMC2305</t>
+  </si>
+  <si>
+    <t>EMC2305-1-AP-CT-ND</t>
+  </si>
+  <si>
     <t>EMC2305-1-AP-TR</t>
   </si>
   <si>
-    <t>EMC2305-1-AP-CT-ND</t>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>PCA9546ARGVR</t>
+  </si>
+  <si>
+    <t>296-21771-1-ND</t>
   </si>
   <si>
     <t>Y1</t>
@@ -732,19 +789,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.6640625" customWidth="1"/>
     <col min="2" max="5" width="30.6640625" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -760,481 +818,597 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>11</v>
-      </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="E5" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2</v>
       </c>
       <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>26</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
         <v>29</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>30</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>31</v>
       </c>
-      <c r="E8" t="s">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>33</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>34</v>
       </c>
-      <c r="D9" t="s">
-        <v>35</v>
-      </c>
       <c r="E9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
       <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
         <v>36</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>37</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>38</v>
       </c>
-      <c r="E10" t="s">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>40</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>41</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>42</v>
       </c>
-      <c r="E11" t="s">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>44</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>45</v>
       </c>
-      <c r="D12" t="s">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
         <v>46</v>
       </c>
-      <c r="E12" t="s">
+      <c r="C13" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
         <v>48</v>
       </c>
-      <c r="C13" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" t="s">
-        <v>50</v>
-      </c>
       <c r="E13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>4</v>
       </c>
       <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
         <v>51</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
         <v>52</v>
       </c>
-      <c r="D14" t="s">
+      <c r="C15" t="s">
         <v>53</v>
       </c>
-      <c r="E14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
         <v>54</v>
       </c>
-      <c r="C15" t="s">
+      <c r="E15" t="s">
         <v>55</v>
       </c>
-      <c r="D15" t="s">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
         <v>56</v>
       </c>
-      <c r="E15" t="s">
+      <c r="C16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21">
         <v>2</v>
       </c>
-      <c r="B16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" t="s">
-        <v>63</v>
-      </c>
-      <c r="E17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="B21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
         <v>3</v>
       </c>
-      <c r="B18" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="B23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24">
         <v>2</v>
       </c>
-      <c r="B19" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" t="s">
-        <v>69</v>
-      </c>
-      <c r="D19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" t="s">
-        <v>73</v>
-      </c>
-      <c r="D20" t="s">
-        <v>74</v>
-      </c>
-      <c r="E20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>3</v>
-      </c>
-      <c r="B21" t="s">
-        <v>76</v>
-      </c>
-      <c r="C21" t="s">
-        <v>77</v>
-      </c>
-      <c r="D21" t="s">
-        <v>78</v>
-      </c>
-      <c r="E21" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>2</v>
-      </c>
-      <c r="B22" t="s">
-        <v>80</v>
-      </c>
-      <c r="C22" t="s">
-        <v>81</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="B24" t="s">
         <v>82</v>
       </c>
-      <c r="E22" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="C24" t="s">
         <v>83</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D24" t="s">
         <v>84</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E24" t="s">
         <v>85</v>
       </c>
-      <c r="E23" t="s">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="C25" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
         <v>4</v>
       </c>
-      <c r="B24" t="s">
-        <v>87</v>
-      </c>
-      <c r="C24" t="s">
-        <v>88</v>
-      </c>
-      <c r="D24" t="s">
-        <v>89</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="B26" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>1</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="C26" t="s">
         <v>91</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D26" t="s">
         <v>92</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E26" t="s">
         <v>93</v>
       </c>
-      <c r="E25" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>1</v>
-      </c>
-      <c r="B26" t="s">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
         <v>94</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>95</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>96</v>
       </c>
-      <c r="E26" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="E27" t="s">
         <v>97</v>
       </c>
-      <c r="C27" t="s">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
         <v>98</v>
       </c>
-      <c r="D27" t="s">
+      <c r="C28" t="s">
         <v>99</v>
       </c>
-      <c r="E27" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="D28" t="s">
         <v>100</v>
-      </c>
-      <c r="C28" t="s">
-        <v>101</v>
-      </c>
-      <c r="D28" t="s">
-        <v>102</v>
       </c>
       <c r="E28" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
       <c r="B29" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" t="s">
         <v>103</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>9</v>
+      </c>
+      <c r="B30" t="s">
         <v>104</v>
       </c>
-      <c r="D29" t="s">
+      <c r="C30" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" t="s">
+        <v>68</v>
+      </c>
+      <c r="E30" t="s">
+        <v>69</v>
+      </c>
+      <c r="F30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
         <v>105</v>
       </c>
-      <c r="E29" t="s">
+      <c r="C31" t="s">
         <v>106</v>
+      </c>
+      <c r="D31" t="s">
+        <v>107</v>
+      </c>
+      <c r="E31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>109</v>
+      </c>
+      <c r="C32" t="s">
+        <v>110</v>
+      </c>
+      <c r="D32" t="s">
+        <v>111</v>
+      </c>
+      <c r="E32" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>112</v>
+      </c>
+      <c r="C33" t="s">
+        <v>113</v>
+      </c>
+      <c r="D33" t="s">
+        <v>114</v>
+      </c>
+      <c r="E33" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" t="s">
+        <v>116</v>
+      </c>
+      <c r="D34" t="s">
+        <v>117</v>
+      </c>
+      <c r="E34" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>119</v>
+      </c>
+      <c r="C35" t="s">
+        <v>120</v>
+      </c>
+      <c r="D35" t="s">
+        <v>121</v>
+      </c>
+      <c r="E35" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>122</v>
+      </c>
+      <c r="C36" t="s">
+        <v>123</v>
+      </c>
+      <c r="D36" t="s">
+        <v>124</v>
+      </c>
+      <c r="E36" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1244,7 +1418,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1270,10 +1444,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1281,21 +1455,21 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1303,10 +1477,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1314,10 +1488,10 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1325,10 +1499,10 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1336,10 +1510,10 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1347,10 +1521,10 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1358,10 +1532,10 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1369,10 +1543,10 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1380,10 +1554,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1391,10 +1562,10 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
         <v>48</v>
-      </c>
-      <c r="C13" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1402,10 +1573,10 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
         <v>51</v>
-      </c>
-      <c r="C14" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1413,21 +1584,18 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
         <v>54</v>
-      </c>
-      <c r="C15" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1435,87 +1603,84 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C19" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C20" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C21" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C23" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C24" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -1523,21 +1688,21 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C25" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C26" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -1545,10 +1710,10 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -1556,10 +1721,10 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" t="s">
         <v>100</v>
-      </c>
-      <c r="C28" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -1567,10 +1732,76 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
         <v>105</v>
+      </c>
+      <c r="C30" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>119</v>
+      </c>
+      <c r="C34" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>122</v>
+      </c>
+      <c r="C35" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>